<commit_message>
Continuação do desenvolvimento do trabalho - entrega 2.
</commit_message>
<xml_diff>
--- a/forecasting.xlsx
+++ b/forecasting.xlsx
@@ -157,19 +157,19 @@
         <v>265.8220835637547</v>
       </c>
       <c r="C2" t="n">
-        <v>1414.601696847661</v>
+        <v>1555.0202227272803</v>
       </c>
       <c r="D2" t="n">
         <v>910.9916666672841</v>
       </c>
       <c r="E2" t="n">
-        <v>1708.5978699103107</v>
+        <v>1728.048453880696</v>
       </c>
       <c r="F2" t="n">
         <v>1129.1105086842804</v>
       </c>
       <c r="G2" t="n">
-        <v>926.4590393949422</v>
+        <v>857.0062033087174</v>
       </c>
       <c r="H2" t="n">
         <v>431.9427142739812</v>
@@ -178,7 +178,7 @@
         <v>2006.3999999999999</v>
       </c>
       <c r="J2" t="n">
-        <v>467.29214557835206</v>
+        <v>486.18848614453566</v>
       </c>
     </row>
     <row r="3">
@@ -189,19 +189,19 @@
         <v>231.47411461542777</v>
       </c>
       <c r="C3" t="n">
-        <v>1125.5132511174008</v>
+        <v>1164.3187227451722</v>
       </c>
       <c r="D3" t="n">
         <v>1030.5916666672842</v>
       </c>
       <c r="E3" t="n">
-        <v>1797.2264778489398</v>
+        <v>1775.1351688050452</v>
       </c>
       <c r="F3" t="n">
         <v>974.0274650561599</v>
       </c>
       <c r="G3" t="n">
-        <v>1200.6263903418549</v>
+        <v>1132.8234137597165</v>
       </c>
       <c r="H3" t="n">
         <v>493.07379574787274</v>
@@ -210,7 +210,7 @@
         <v>2448.0</v>
       </c>
       <c r="J3" t="n">
-        <v>543.4744280737973</v>
+        <v>520.4790379943112</v>
       </c>
     </row>
     <row r="4">
@@ -221,19 +221,19 @@
         <v>228.6782640348942</v>
       </c>
       <c r="C4" t="n">
-        <v>1099.317814884688</v>
+        <v>1082.2497654902295</v>
       </c>
       <c r="D4" t="n">
         <v>1414.6916666672842</v>
       </c>
       <c r="E4" t="n">
-        <v>1808.3505007739373</v>
+        <v>1790.0636351976775</v>
       </c>
       <c r="F4" t="n">
         <v>1061.109414226235</v>
       </c>
       <c r="G4" t="n">
-        <v>801.1739481932163</v>
+        <v>1214.5579814865614</v>
       </c>
       <c r="H4" t="n">
         <v>565.468436620452</v>
@@ -242,7 +242,7 @@
         <v>2606.4</v>
       </c>
       <c r="J4" t="n">
-        <v>881.4357832581213</v>
+        <v>857.9446082559186</v>
       </c>
     </row>
     <row r="5">
@@ -253,19 +253,19 @@
         <v>240.97125593663986</v>
       </c>
       <c r="C5" t="n">
-        <v>1090.501439273488</v>
+        <v>1098.2061537285508</v>
       </c>
       <c r="D5" t="n">
         <v>1281.291666667284</v>
       </c>
       <c r="E5" t="n">
-        <v>1793.2853035886862</v>
+        <v>1783.106531266468</v>
       </c>
       <c r="F5" t="n">
         <v>1592.6078673862035</v>
       </c>
       <c r="G5" t="n">
-        <v>888.3016094200791</v>
+        <v>1231.7317987479455</v>
       </c>
       <c r="H5" t="n">
         <v>612.5205824020809</v>
@@ -274,7 +274,7 @@
         <v>3417.6</v>
       </c>
       <c r="J5" t="n">
-        <v>698.716123562112</v>
+        <v>716.0666605380537</v>
       </c>
     </row>
     <row r="6">
@@ -285,19 +285,19 @@
         <v>211.923027939451</v>
       </c>
       <c r="C6" t="n">
-        <v>549.6738418883855</v>
+        <v>670.6704228077194</v>
       </c>
       <c r="D6" t="n">
         <v>1053.591666667284</v>
       </c>
       <c r="E6" t="n">
-        <v>1793.371470500333</v>
+        <v>1834.5173487132</v>
       </c>
       <c r="F6" t="n">
         <v>1359.4037281431526</v>
       </c>
       <c r="G6" t="n">
-        <v>778.4743612875615</v>
+        <v>852.9814888185717</v>
       </c>
       <c r="H6" t="n">
         <v>396.51214600691935</v>
@@ -306,7 +306,7 @@
         <v>2448.0</v>
       </c>
       <c r="J6" t="n">
-        <v>419.6916189018216</v>
+        <v>324.4553828666919</v>
       </c>
     </row>
     <row r="7">
@@ -317,19 +317,19 @@
         <v>203.22059343149252</v>
       </c>
       <c r="C7" t="n">
-        <v>733.8557265521245</v>
+        <v>796.598077660808</v>
       </c>
       <c r="D7" t="n">
         <v>768.391666667284</v>
       </c>
       <c r="E7" t="n">
-        <v>1716.9837744807212</v>
+        <v>1728.8773409661192</v>
       </c>
       <c r="F7" t="n">
         <v>1285.071229462075</v>
       </c>
       <c r="G7" t="n">
-        <v>911.746609729425</v>
+        <v>760.4505100067738</v>
       </c>
       <c r="H7" t="n">
         <v>379.52008021661925</v>
@@ -338,7 +338,7 @@
         <v>2352.0</v>
       </c>
       <c r="J7" t="n">
-        <v>536.1677041524703</v>
+        <v>519.9936765819638</v>
       </c>
     </row>
     <row r="8">
@@ -349,19 +349,19 @@
         <v>188.36557241939929</v>
       </c>
       <c r="C8" t="n">
-        <v>923.6189314185638</v>
+        <v>895.5350333959236</v>
       </c>
       <c r="D8" t="n">
         <v>959.2916666672841</v>
       </c>
       <c r="E8" t="n">
-        <v>1782.8215542835458</v>
+        <v>1765.7633332717332</v>
       </c>
       <c r="F8" t="n">
         <v>1587.7659916613786</v>
       </c>
       <c r="G8" t="n">
-        <v>805.7494730414978</v>
+        <v>839.2404773858684</v>
       </c>
       <c r="H8" t="n">
         <v>339.67210138873014</v>
@@ -370,7 +370,7 @@
         <v>1977.6</v>
       </c>
       <c r="J8" t="n">
-        <v>573.2178228723917</v>
+        <v>669.5886649405261</v>
       </c>
     </row>
     <row r="9">
@@ -381,19 +381,19 @@
         <v>186.8233862115498</v>
       </c>
       <c r="C9" t="n">
-        <v>998.7466308098732</v>
+        <v>964.8175737204451</v>
       </c>
       <c r="D9" t="n">
         <v>910.9916666672841</v>
       </c>
       <c r="E9" t="n">
-        <v>1788.3408748105942</v>
+        <v>1801.3261768274165</v>
       </c>
       <c r="F9" t="n">
         <v>1088.8040440673315</v>
       </c>
       <c r="G9" t="n">
-        <v>1115.2892642316667</v>
+        <v>873.0961706878122</v>
       </c>
       <c r="H9" t="n">
         <v>286.7495819195926</v>
@@ -402,7 +402,7 @@
         <v>1963.1999999999998</v>
       </c>
       <c r="J9" t="n">
-        <v>1097.5781059746964</v>
+        <v>895.2119711246548</v>
       </c>
     </row>
     <row r="10">
@@ -413,19 +413,19 @@
         <v>221.3196647041807</v>
       </c>
       <c r="C10" t="n">
-        <v>1051.5376550305562</v>
+        <v>1101.2542918970034</v>
       </c>
       <c r="D10" t="n">
         <v>881.0916666672841</v>
       </c>
       <c r="E10" t="n">
-        <v>1907.642299338299</v>
+        <v>1759.000019339333</v>
       </c>
       <c r="F10" t="n">
         <v>984.4482394621131</v>
       </c>
       <c r="G10" t="n">
-        <v>766.544776718578</v>
+        <v>717.4237074094106</v>
       </c>
       <c r="H10" t="n">
         <v>253.17583269436943</v>
@@ -434,7 +434,7 @@
         <v>1886.3999999999999</v>
       </c>
       <c r="J10" t="n">
-        <v>727.4392743003291</v>
+        <v>736.942226335113</v>
       </c>
     </row>
     <row r="11">
@@ -445,19 +445,19 @@
         <v>259.74386690940736</v>
       </c>
       <c r="C11" t="n">
-        <v>1140.6908715781885</v>
+        <v>1193.063143001388</v>
       </c>
       <c r="D11" t="n">
         <v>759.1916666672842</v>
       </c>
       <c r="E11" t="n">
-        <v>1716.3361765934173</v>
+        <v>1731.8612229692724</v>
       </c>
       <c r="F11" t="n">
         <v>980.7200871510814</v>
       </c>
       <c r="G11" t="n">
-        <v>492.2388288373787</v>
+        <v>763.1204121440577</v>
       </c>
       <c r="H11" t="n">
         <v>224.73396243092412</v>
@@ -466,7 +466,7 @@
         <v>1411.2</v>
       </c>
       <c r="J11" t="n">
-        <v>529.428426744444</v>
+        <v>534.0247059132386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalização da Entrega 2.
</commit_message>
<xml_diff>
--- a/forecasting.xlsx
+++ b/forecasting.xlsx
@@ -157,13 +157,13 @@
         <v>265.8220835637547</v>
       </c>
       <c r="C2" t="n">
-        <v>1555.0202227272803</v>
+        <v>1434.7237589384115</v>
       </c>
       <c r="D2" t="n">
         <v>910.9916666672841</v>
       </c>
       <c r="E2" t="n">
-        <v>1728.048453880696</v>
+        <v>1727.5359942936627</v>
       </c>
       <c r="F2" t="n">
         <v>1129.1105086842804</v>
@@ -178,7 +178,7 @@
         <v>2006.3999999999999</v>
       </c>
       <c r="J2" t="n">
-        <v>486.18848614453566</v>
+        <v>471.96269851437467</v>
       </c>
     </row>
     <row r="3">
@@ -189,13 +189,13 @@
         <v>231.47411461542777</v>
       </c>
       <c r="C3" t="n">
-        <v>1164.3187227451722</v>
+        <v>1090.0368042981816</v>
       </c>
       <c r="D3" t="n">
         <v>1030.5916666672842</v>
       </c>
       <c r="E3" t="n">
-        <v>1775.1351688050452</v>
+        <v>1761.269001654387</v>
       </c>
       <c r="F3" t="n">
         <v>974.0274650561599</v>
@@ -210,7 +210,7 @@
         <v>2448.0</v>
       </c>
       <c r="J3" t="n">
-        <v>520.4790379943112</v>
+        <v>534.561144794189</v>
       </c>
     </row>
     <row r="4">
@@ -221,13 +221,13 @@
         <v>228.6782640348942</v>
       </c>
       <c r="C4" t="n">
-        <v>1082.2497654902295</v>
+        <v>1091.3452497379058</v>
       </c>
       <c r="D4" t="n">
         <v>1414.6916666672842</v>
       </c>
       <c r="E4" t="n">
-        <v>1790.0636351976775</v>
+        <v>1859.0263156237197</v>
       </c>
       <c r="F4" t="n">
         <v>1061.109414226235</v>
@@ -242,7 +242,7 @@
         <v>2606.4</v>
       </c>
       <c r="J4" t="n">
-        <v>857.9446082559186</v>
+        <v>849.0588754685059</v>
       </c>
     </row>
     <row r="5">
@@ -253,13 +253,13 @@
         <v>240.97125593663986</v>
       </c>
       <c r="C5" t="n">
-        <v>1098.2061537285508</v>
+        <v>1084.9869206170813</v>
       </c>
       <c r="D5" t="n">
         <v>1281.291666667284</v>
       </c>
       <c r="E5" t="n">
-        <v>1783.106531266468</v>
+        <v>1883.4933627092037</v>
       </c>
       <c r="F5" t="n">
         <v>1592.6078673862035</v>
@@ -274,7 +274,7 @@
         <v>3417.6</v>
       </c>
       <c r="J5" t="n">
-        <v>716.0666605380537</v>
+        <v>719.2840458466168</v>
       </c>
     </row>
     <row r="6">
@@ -285,13 +285,13 @@
         <v>211.923027939451</v>
       </c>
       <c r="C6" t="n">
-        <v>670.6704228077194</v>
+        <v>583.9977800533463</v>
       </c>
       <c r="D6" t="n">
         <v>1053.591666667284</v>
       </c>
       <c r="E6" t="n">
-        <v>1834.5173487132</v>
+        <v>1985.1420231656718</v>
       </c>
       <c r="F6" t="n">
         <v>1359.4037281431526</v>
@@ -306,7 +306,7 @@
         <v>2448.0</v>
       </c>
       <c r="J6" t="n">
-        <v>324.4553828666919</v>
+        <v>356.53577602764267</v>
       </c>
     </row>
     <row r="7">
@@ -317,13 +317,13 @@
         <v>203.22059343149252</v>
       </c>
       <c r="C7" t="n">
-        <v>796.598077660808</v>
+        <v>818.0998139706464</v>
       </c>
       <c r="D7" t="n">
         <v>768.391666667284</v>
       </c>
       <c r="E7" t="n">
-        <v>1728.8773409661192</v>
+        <v>1729.864018678907</v>
       </c>
       <c r="F7" t="n">
         <v>1285.071229462075</v>
@@ -338,7 +338,7 @@
         <v>2352.0</v>
       </c>
       <c r="J7" t="n">
-        <v>519.9936765819638</v>
+        <v>532.4200212299824</v>
       </c>
     </row>
     <row r="8">
@@ -349,13 +349,13 @@
         <v>188.36557241939929</v>
       </c>
       <c r="C8" t="n">
-        <v>895.5350333959236</v>
+        <v>939.2589368041106</v>
       </c>
       <c r="D8" t="n">
         <v>959.2916666672841</v>
       </c>
       <c r="E8" t="n">
-        <v>1765.7633332717332</v>
+        <v>1705.2557394324979</v>
       </c>
       <c r="F8" t="n">
         <v>1587.7659916613786</v>
@@ -370,7 +370,7 @@
         <v>1977.6</v>
       </c>
       <c r="J8" t="n">
-        <v>669.5886649405261</v>
+        <v>647.3504003121201</v>
       </c>
     </row>
     <row r="9">
@@ -381,13 +381,13 @@
         <v>186.8233862115498</v>
       </c>
       <c r="C9" t="n">
-        <v>964.8175737204451</v>
+        <v>993.5273242633199</v>
       </c>
       <c r="D9" t="n">
         <v>910.9916666672841</v>
       </c>
       <c r="E9" t="n">
-        <v>1801.3261768274165</v>
+        <v>1762.7113861234513</v>
       </c>
       <c r="F9" t="n">
         <v>1088.8040440673315</v>
@@ -402,7 +402,7 @@
         <v>1963.1999999999998</v>
       </c>
       <c r="J9" t="n">
-        <v>895.2119711246548</v>
+        <v>951.9623051755061</v>
       </c>
     </row>
     <row r="10">
@@ -413,13 +413,13 @@
         <v>221.3196647041807</v>
       </c>
       <c r="C10" t="n">
-        <v>1101.2542918970034</v>
+        <v>1057.7232374961402</v>
       </c>
       <c r="D10" t="n">
         <v>881.0916666672841</v>
       </c>
       <c r="E10" t="n">
-        <v>1759.000019339333</v>
+        <v>2045.9363133819963</v>
       </c>
       <c r="F10" t="n">
         <v>984.4482394621131</v>
@@ -434,7 +434,7 @@
         <v>1886.3999999999999</v>
       </c>
       <c r="J10" t="n">
-        <v>736.942226335113</v>
+        <v>727.0181732426795</v>
       </c>
     </row>
     <row r="11">
@@ -445,13 +445,13 @@
         <v>259.74386690940736</v>
       </c>
       <c r="C11" t="n">
-        <v>1193.063143001388</v>
+        <v>1208.5769622812456</v>
       </c>
       <c r="D11" t="n">
         <v>759.1916666672842</v>
       </c>
       <c r="E11" t="n">
-        <v>1731.8612229692724</v>
+        <v>1733.641494546538</v>
       </c>
       <c r="F11" t="n">
         <v>980.7200871510814</v>
@@ -466,7 +466,7 @@
         <v>1411.2</v>
       </c>
       <c r="J11" t="n">
-        <v>534.0247059132386</v>
+        <v>533.938009398067</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Entrega 3 - Nível de Serviço e Estoque.
</commit_message>
<xml_diff>
--- a/forecasting.xlsx
+++ b/forecasting.xlsx
@@ -157,19 +157,19 @@
         <v>265.8220835637547</v>
       </c>
       <c r="C2" t="n">
-        <v>1434.7237589384115</v>
+        <v>1440.690759875038</v>
       </c>
       <c r="D2" t="n">
         <v>910.9916666672841</v>
       </c>
       <c r="E2" t="n">
-        <v>1727.5359942936627</v>
+        <v>1707.8679159935714</v>
       </c>
       <c r="F2" t="n">
         <v>1129.1105086842804</v>
       </c>
       <c r="G2" t="n">
-        <v>857.0062033087174</v>
+        <v>955.5854869749402</v>
       </c>
       <c r="H2" t="n">
         <v>431.9427142739812</v>
@@ -178,7 +178,7 @@
         <v>2006.3999999999999</v>
       </c>
       <c r="J2" t="n">
-        <v>471.96269851437467</v>
+        <v>488.54336074569926</v>
       </c>
     </row>
     <row r="3">
@@ -189,19 +189,19 @@
         <v>231.47411461542777</v>
       </c>
       <c r="C3" t="n">
-        <v>1090.0368042981816</v>
+        <v>1102.6446499341537</v>
       </c>
       <c r="D3" t="n">
         <v>1030.5916666672842</v>
       </c>
       <c r="E3" t="n">
-        <v>1761.269001654387</v>
+        <v>1822.2997128583345</v>
       </c>
       <c r="F3" t="n">
         <v>974.0274650561599</v>
       </c>
       <c r="G3" t="n">
-        <v>1132.8234137597165</v>
+        <v>1194.1015187255632</v>
       </c>
       <c r="H3" t="n">
         <v>493.07379574787274</v>
@@ -210,7 +210,7 @@
         <v>2448.0</v>
       </c>
       <c r="J3" t="n">
-        <v>534.561144794189</v>
+        <v>519.3330594676355</v>
       </c>
     </row>
     <row r="4">
@@ -221,19 +221,19 @@
         <v>228.6782640348942</v>
       </c>
       <c r="C4" t="n">
-        <v>1091.3452497379058</v>
+        <v>1112.3315134753032</v>
       </c>
       <c r="D4" t="n">
         <v>1414.6916666672842</v>
       </c>
       <c r="E4" t="n">
-        <v>1859.0263156237197</v>
+        <v>2035.6893118204573</v>
       </c>
       <c r="F4" t="n">
         <v>1061.109414226235</v>
       </c>
       <c r="G4" t="n">
-        <v>1214.5579814865614</v>
+        <v>799.1835329027557</v>
       </c>
       <c r="H4" t="n">
         <v>565.468436620452</v>
@@ -242,7 +242,7 @@
         <v>2606.4</v>
       </c>
       <c r="J4" t="n">
-        <v>849.0588754685059</v>
+        <v>811.4804669414951</v>
       </c>
     </row>
     <row r="5">
@@ -253,19 +253,19 @@
         <v>240.97125593663986</v>
       </c>
       <c r="C5" t="n">
-        <v>1084.9869206170813</v>
+        <v>1100.2900609715684</v>
       </c>
       <c r="D5" t="n">
         <v>1281.291666667284</v>
       </c>
       <c r="E5" t="n">
-        <v>1883.4933627092037</v>
+        <v>1722.9788873957802</v>
       </c>
       <c r="F5" t="n">
         <v>1592.6078673862035</v>
       </c>
       <c r="G5" t="n">
-        <v>1231.7317987479455</v>
+        <v>895.2177544738933</v>
       </c>
       <c r="H5" t="n">
         <v>612.5205824020809</v>
@@ -274,7 +274,7 @@
         <v>3417.6</v>
       </c>
       <c r="J5" t="n">
-        <v>719.2840458466168</v>
+        <v>739.349160139947</v>
       </c>
     </row>
     <row r="6">
@@ -285,19 +285,19 @@
         <v>211.923027939451</v>
       </c>
       <c r="C6" t="n">
-        <v>583.9977800533463</v>
+        <v>546.5450380717565</v>
       </c>
       <c r="D6" t="n">
         <v>1053.591666667284</v>
       </c>
       <c r="E6" t="n">
-        <v>1985.1420231656718</v>
+        <v>1931.5995437187648</v>
       </c>
       <c r="F6" t="n">
         <v>1359.4037281431526</v>
       </c>
       <c r="G6" t="n">
-        <v>852.9814888185717</v>
+        <v>741.3650300668102</v>
       </c>
       <c r="H6" t="n">
         <v>396.51214600691935</v>
@@ -306,7 +306,7 @@
         <v>2448.0</v>
       </c>
       <c r="J6" t="n">
-        <v>356.53577602764267</v>
+        <v>152.5266386930083</v>
       </c>
     </row>
     <row r="7">
@@ -317,19 +317,19 @@
         <v>203.22059343149252</v>
       </c>
       <c r="C7" t="n">
-        <v>818.0998139706464</v>
+        <v>801.8704103813825</v>
       </c>
       <c r="D7" t="n">
         <v>768.391666667284</v>
       </c>
       <c r="E7" t="n">
-        <v>1729.864018678907</v>
+        <v>1713.9983884607057</v>
       </c>
       <c r="F7" t="n">
         <v>1285.071229462075</v>
       </c>
       <c r="G7" t="n">
-        <v>760.4505100067738</v>
+        <v>708.4912224940716</v>
       </c>
       <c r="H7" t="n">
         <v>379.52008021661925</v>
@@ -338,7 +338,7 @@
         <v>2352.0</v>
       </c>
       <c r="J7" t="n">
-        <v>532.4200212299824</v>
+        <v>516.8625075072472</v>
       </c>
     </row>
     <row r="8">
@@ -349,19 +349,19 @@
         <v>188.36557241939929</v>
       </c>
       <c r="C8" t="n">
-        <v>939.2589368041106</v>
+        <v>929.5909822242468</v>
       </c>
       <c r="D8" t="n">
         <v>959.2916666672841</v>
       </c>
       <c r="E8" t="n">
-        <v>1705.2557394324979</v>
+        <v>1884.9234449812907</v>
       </c>
       <c r="F8" t="n">
         <v>1587.7659916613786</v>
       </c>
       <c r="G8" t="n">
-        <v>839.2404773858684</v>
+        <v>701.1341987630879</v>
       </c>
       <c r="H8" t="n">
         <v>339.67210138873014</v>
@@ -370,7 +370,7 @@
         <v>1977.6</v>
       </c>
       <c r="J8" t="n">
-        <v>647.3504003121201</v>
+        <v>698.1750159023352</v>
       </c>
     </row>
     <row r="9">
@@ -381,19 +381,19 @@
         <v>186.8233862115498</v>
       </c>
       <c r="C9" t="n">
-        <v>993.5273242633199</v>
+        <v>969.4593980148438</v>
       </c>
       <c r="D9" t="n">
         <v>910.9916666672841</v>
       </c>
       <c r="E9" t="n">
-        <v>1762.7113861234513</v>
+        <v>1869.9693203495092</v>
       </c>
       <c r="F9" t="n">
         <v>1088.8040440673315</v>
       </c>
       <c r="G9" t="n">
-        <v>873.0961706878122</v>
+        <v>743.9308036328167</v>
       </c>
       <c r="H9" t="n">
         <v>286.7495819195926</v>
@@ -402,7 +402,7 @@
         <v>1963.1999999999998</v>
       </c>
       <c r="J9" t="n">
-        <v>951.9623051755061</v>
+        <v>818.8938606109518</v>
       </c>
     </row>
     <row r="10">
@@ -413,19 +413,19 @@
         <v>221.3196647041807</v>
       </c>
       <c r="C10" t="n">
-        <v>1057.7232374961402</v>
+        <v>1059.773744490573</v>
       </c>
       <c r="D10" t="n">
         <v>881.0916666672841</v>
       </c>
       <c r="E10" t="n">
-        <v>2045.9363133819963</v>
+        <v>2510.7021607639144</v>
       </c>
       <c r="F10" t="n">
         <v>984.4482394621131</v>
       </c>
       <c r="G10" t="n">
-        <v>717.4237074094106</v>
+        <v>858.83915007571</v>
       </c>
       <c r="H10" t="n">
         <v>253.17583269436943</v>
@@ -434,7 +434,7 @@
         <v>1886.3999999999999</v>
       </c>
       <c r="J10" t="n">
-        <v>727.0181732426795</v>
+        <v>778.1921690866949</v>
       </c>
     </row>
     <row r="11">
@@ -445,19 +445,19 @@
         <v>259.74386690940736</v>
       </c>
       <c r="C11" t="n">
-        <v>1208.5769622812456</v>
+        <v>1142.2503670735578</v>
       </c>
       <c r="D11" t="n">
         <v>759.1916666672842</v>
       </c>
       <c r="E11" t="n">
-        <v>1733.641494546538</v>
+        <v>1705.1364138896488</v>
       </c>
       <c r="F11" t="n">
         <v>980.7200871510814</v>
       </c>
       <c r="G11" t="n">
-        <v>763.1204121440577</v>
+        <v>753.2402760522962</v>
       </c>
       <c r="H11" t="n">
         <v>224.73396243092412</v>
@@ -466,7 +466,7 @@
         <v>1411.2</v>
       </c>
       <c r="J11" t="n">
-        <v>533.938009398067</v>
+        <v>707.7514220216078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correções e início da entrega 4.
</commit_message>
<xml_diff>
--- a/forecasting.xlsx
+++ b/forecasting.xlsx
@@ -157,19 +157,19 @@
         <v>265.8220835637547</v>
       </c>
       <c r="C2" t="n">
-        <v>1440.690759875038</v>
+        <v>1514.7329694126095</v>
       </c>
       <c r="D2" t="n">
         <v>910.9916666672841</v>
       </c>
       <c r="E2" t="n">
-        <v>1707.8679159935714</v>
+        <v>1731.0115884581783</v>
       </c>
       <c r="F2" t="n">
         <v>1129.1105086842804</v>
       </c>
       <c r="G2" t="n">
-        <v>955.5854869749402</v>
+        <v>957.2368372616152</v>
       </c>
       <c r="H2" t="n">
         <v>431.9427142739812</v>
@@ -178,7 +178,7 @@
         <v>2006.3999999999999</v>
       </c>
       <c r="J2" t="n">
-        <v>488.54336074569926</v>
+        <v>471.2227821772243</v>
       </c>
     </row>
     <row r="3">
@@ -189,19 +189,19 @@
         <v>231.47411461542777</v>
       </c>
       <c r="C3" t="n">
-        <v>1102.6446499341537</v>
+        <v>1060.1522125646386</v>
       </c>
       <c r="D3" t="n">
         <v>1030.5916666672842</v>
       </c>
       <c r="E3" t="n">
-        <v>1822.2997128583345</v>
+        <v>1813.0016146387984</v>
       </c>
       <c r="F3" t="n">
         <v>974.0274650561599</v>
       </c>
       <c r="G3" t="n">
-        <v>1194.1015187255632</v>
+        <v>1137.1588884089708</v>
       </c>
       <c r="H3" t="n">
         <v>493.07379574787274</v>
@@ -210,7 +210,7 @@
         <v>2448.0</v>
       </c>
       <c r="J3" t="n">
-        <v>519.3330594676355</v>
+        <v>537.1585582369928</v>
       </c>
     </row>
     <row r="4">
@@ -221,19 +221,19 @@
         <v>228.6782640348942</v>
       </c>
       <c r="C4" t="n">
-        <v>1112.3315134753032</v>
+        <v>1089.1068138559324</v>
       </c>
       <c r="D4" t="n">
         <v>1414.6916666672842</v>
       </c>
       <c r="E4" t="n">
-        <v>2035.6893118204573</v>
+        <v>1791.6388159567416</v>
       </c>
       <c r="F4" t="n">
         <v>1061.109414226235</v>
       </c>
       <c r="G4" t="n">
-        <v>799.1835329027557</v>
+        <v>825.6203014835611</v>
       </c>
       <c r="H4" t="n">
         <v>565.468436620452</v>
@@ -242,7 +242,7 @@
         <v>2606.4</v>
       </c>
       <c r="J4" t="n">
-        <v>811.4804669414951</v>
+        <v>880.0915727635413</v>
       </c>
     </row>
     <row r="5">
@@ -253,19 +253,19 @@
         <v>240.97125593663986</v>
       </c>
       <c r="C5" t="n">
-        <v>1100.2900609715684</v>
+        <v>1085.5815223093905</v>
       </c>
       <c r="D5" t="n">
         <v>1281.291666667284</v>
       </c>
       <c r="E5" t="n">
-        <v>1722.9788873957802</v>
+        <v>1821.7586330497975</v>
       </c>
       <c r="F5" t="n">
         <v>1592.6078673862035</v>
       </c>
       <c r="G5" t="n">
-        <v>895.2177544738933</v>
+        <v>1082.9627095654841</v>
       </c>
       <c r="H5" t="n">
         <v>612.5205824020809</v>
@@ -274,7 +274,7 @@
         <v>3417.6</v>
       </c>
       <c r="J5" t="n">
-        <v>739.349160139947</v>
+        <v>713.237348637963</v>
       </c>
     </row>
     <row r="6">
@@ -285,19 +285,19 @@
         <v>211.923027939451</v>
       </c>
       <c r="C6" t="n">
-        <v>546.5450380717565</v>
+        <v>659.9592090102584</v>
       </c>
       <c r="D6" t="n">
         <v>1053.591666667284</v>
       </c>
       <c r="E6" t="n">
-        <v>1931.5995437187648</v>
+        <v>1908.8819777038418</v>
       </c>
       <c r="F6" t="n">
         <v>1359.4037281431526</v>
       </c>
       <c r="G6" t="n">
-        <v>741.3650300668102</v>
+        <v>805.8749150451886</v>
       </c>
       <c r="H6" t="n">
         <v>396.51214600691935</v>
@@ -306,7 +306,7 @@
         <v>2448.0</v>
       </c>
       <c r="J6" t="n">
-        <v>152.5266386930083</v>
+        <v>403.8818631413123</v>
       </c>
     </row>
     <row r="7">
@@ -317,19 +317,19 @@
         <v>203.22059343149252</v>
       </c>
       <c r="C7" t="n">
-        <v>801.8704103813825</v>
+        <v>814.5043961409763</v>
       </c>
       <c r="D7" t="n">
         <v>768.391666667284</v>
       </c>
       <c r="E7" t="n">
-        <v>1713.9983884607057</v>
+        <v>1732.2522243302978</v>
       </c>
       <c r="F7" t="n">
         <v>1285.071229462075</v>
       </c>
       <c r="G7" t="n">
-        <v>708.4912224940716</v>
+        <v>874.550102548951</v>
       </c>
       <c r="H7" t="n">
         <v>379.52008021661925</v>
@@ -338,7 +338,7 @@
         <v>2352.0</v>
       </c>
       <c r="J7" t="n">
-        <v>516.8625075072472</v>
+        <v>538.049241798567</v>
       </c>
     </row>
     <row r="8">
@@ -349,19 +349,19 @@
         <v>188.36557241939929</v>
       </c>
       <c r="C8" t="n">
-        <v>929.5909822242468</v>
+        <v>902.8117247435255</v>
       </c>
       <c r="D8" t="n">
         <v>959.2916666672841</v>
       </c>
       <c r="E8" t="n">
-        <v>1884.9234449812907</v>
+        <v>1755.6532004432918</v>
       </c>
       <c r="F8" t="n">
         <v>1587.7659916613786</v>
       </c>
       <c r="G8" t="n">
-        <v>701.1341987630879</v>
+        <v>914.2163279336471</v>
       </c>
       <c r="H8" t="n">
         <v>339.67210138873014</v>
@@ -370,7 +370,7 @@
         <v>1977.6</v>
       </c>
       <c r="J8" t="n">
-        <v>698.1750159023352</v>
+        <v>606.4236026044599</v>
       </c>
     </row>
     <row r="9">
@@ -381,19 +381,19 @@
         <v>186.8233862115498</v>
       </c>
       <c r="C9" t="n">
-        <v>969.4593980148438</v>
+        <v>964.2669056735263</v>
       </c>
       <c r="D9" t="n">
         <v>910.9916666672841</v>
       </c>
       <c r="E9" t="n">
-        <v>1869.9693203495092</v>
+        <v>1823.0980967187024</v>
       </c>
       <c r="F9" t="n">
         <v>1088.8040440673315</v>
       </c>
       <c r="G9" t="n">
-        <v>743.9308036328167</v>
+        <v>989.2700660622756</v>
       </c>
       <c r="H9" t="n">
         <v>286.7495819195926</v>
@@ -402,7 +402,7 @@
         <v>1963.1999999999998</v>
       </c>
       <c r="J9" t="n">
-        <v>818.8938606109518</v>
+        <v>1120.6318661902958</v>
       </c>
     </row>
     <row r="10">
@@ -413,19 +413,19 @@
         <v>221.3196647041807</v>
       </c>
       <c r="C10" t="n">
-        <v>1059.773744490573</v>
+        <v>1081.3982042134373</v>
       </c>
       <c r="D10" t="n">
         <v>881.0916666672841</v>
       </c>
       <c r="E10" t="n">
-        <v>2510.7021607639144</v>
+        <v>1758.7518930502324</v>
       </c>
       <c r="F10" t="n">
         <v>984.4482394621131</v>
       </c>
       <c r="G10" t="n">
-        <v>858.83915007571</v>
+        <v>777.6856690849313</v>
       </c>
       <c r="H10" t="n">
         <v>253.17583269436943</v>
@@ -434,7 +434,7 @@
         <v>1886.3999999999999</v>
       </c>
       <c r="J10" t="n">
-        <v>778.1921690866949</v>
+        <v>675.8701970175887</v>
       </c>
     </row>
     <row r="11">
@@ -445,19 +445,19 @@
         <v>259.74386690940736</v>
       </c>
       <c r="C11" t="n">
-        <v>1142.2503670735578</v>
+        <v>1196.5457985170783</v>
       </c>
       <c r="D11" t="n">
         <v>759.1916666672842</v>
       </c>
       <c r="E11" t="n">
-        <v>1705.1364138896488</v>
+        <v>1736.4472428954737</v>
       </c>
       <c r="F11" t="n">
         <v>980.7200871510814</v>
       </c>
       <c r="G11" t="n">
-        <v>753.2402760522962</v>
+        <v>583.147641217855</v>
       </c>
       <c r="H11" t="n">
         <v>224.73396243092412</v>
@@ -466,7 +466,7 @@
         <v>1411.2</v>
       </c>
       <c r="J11" t="n">
-        <v>707.7514220216078</v>
+        <v>537.9952057606333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>